<commit_message>
add search patterns for all vital-signs
</commit_message>
<xml_diff>
--- a/docs/CodeSystem-Ages.xlsx
+++ b/docs/CodeSystem-Ages.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.2.8-beta</t>
+    <t>0.2.9-beta</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-10-20T14:08:50-05:00</t>
+    <t>2022-10-25T15:39:47-05:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
update MIN / MAX values to align with MHV-17222
</commit_message>
<xml_diff>
--- a/docs/CodeSystem-Ages.xlsx
+++ b/docs/CodeSystem-Ages.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.2.9-beta</t>
+    <t>0.2.10-beta</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-02-16T09:21:54-06:00</t>
+    <t>2023-12-06T12:46:33-06:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -347,10 +347,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyFont="true">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true" applyFont="true">
       <alignment vertical="top" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment vertical="top" wrapText="true"/>
     </xf>
   </cellXfs>

</xml_diff>